<commit_message>
removed lx in std, removed ly in 103
</commit_message>
<xml_diff>
--- a/NotchMappingTable.xlsx
+++ b/NotchMappingTable.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\Git\DENSYAGO_OHCPC01A_TO_PS4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7016AAFE-2195-4361-8CE0-9994327B6F64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="28035" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,8 +227,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -569,13 +575,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -587,6 +593,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -633,7 +647,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,9 +679,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,6 +731,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,38 +924,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="10" max="10" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="17.25" thickBot="1"/>
-    <row r="2" spans="2:10">
+    <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="24"/>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="27">
         <v>205</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="22"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="27" t="s">
         <v>36</v>
       </c>
       <c r="I2" s="29"/>
-      <c r="J2" s="27"/>
-    </row>
-    <row r="3" spans="2:10">
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>31</v>
       </c>
@@ -922,7 +972,7 @@
       <c r="G3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="26" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -932,7 +982,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
@@ -955,7 +1005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
@@ -978,7 +1028,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>2</v>
       </c>
@@ -998,10 +1048,10 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>3</v>
       </c>
@@ -1024,7 +1074,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>6</v>
       </c>
@@ -1093,7 +1143,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1166,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>8</v>
       </c>
@@ -1139,7 +1189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1237,7 @@
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1260,7 @@
       </c>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
@@ -1233,7 +1283,7 @@
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>13</v>
       </c>
@@ -1256,7 +1306,7 @@
       </c>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="2:10" ht="17.25" thickBot="1">
+    <row r="18" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
         <v>14</v>
       </c>
@@ -1286,17 +1336,17 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1304,12 +1354,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>